<commit_message>
fixed 2015 buckwheat raw data file: changed year 2105 to 2015 for June 22 dates
</commit_message>
<xml_diff>
--- a/nectar analysis/raw data/2015 Buckwheat Nectar Data v1 original.xlsx
+++ b/nectar analysis/raw data/2015 Buckwheat Nectar Data v1 original.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Audrey McCombs\Desktop\EEB 590\MAL\nectar analysis\raw data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="132" windowWidth="20112" windowHeight="7932"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -386,7 +381,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -421,7 +416,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -632,9 +627,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A435" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V451" sqref="V451"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A175" sqref="A175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6970,7 +6965,7 @@
     </row>
     <row r="140" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A140" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B140">
         <v>0</v>
@@ -7015,7 +7010,7 @@
     </row>
     <row r="141" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A141" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -7060,7 +7055,7 @@
     </row>
     <row r="142" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A142" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -7105,7 +7100,7 @@
     </row>
     <row r="143" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A143" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -7150,7 +7145,7 @@
     </row>
     <row r="144" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A144" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -7195,7 +7190,7 @@
     </row>
     <row r="145" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A145" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B145">
         <v>0</v>
@@ -7240,7 +7235,7 @@
     </row>
     <row r="146" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A146" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -7285,7 +7280,7 @@
     </row>
     <row r="147" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A147" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -7330,7 +7325,7 @@
     </row>
     <row r="148" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A148" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -7381,7 +7376,7 @@
     </row>
     <row r="149" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A149" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -7426,7 +7421,7 @@
     </row>
     <row r="150" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A150" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -7471,7 +7466,7 @@
     </row>
     <row r="151" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A151" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -7516,7 +7511,7 @@
     </row>
     <row r="152" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A152" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -7561,7 +7556,7 @@
     </row>
     <row r="153" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A153" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -7606,7 +7601,7 @@
     </row>
     <row r="154" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A154" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -7651,7 +7646,7 @@
     </row>
     <row r="155" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A155" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -7696,7 +7691,7 @@
     </row>
     <row r="156" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A156" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -7741,7 +7736,7 @@
     </row>
     <row r="157" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A157" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -7786,7 +7781,7 @@
     </row>
     <row r="158" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A158" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -7831,7 +7826,7 @@
     </row>
     <row r="159" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A159" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -7876,7 +7871,7 @@
     </row>
     <row r="160" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A160" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -7921,7 +7916,7 @@
     </row>
     <row r="161" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A161" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -7966,7 +7961,7 @@
     </row>
     <row r="162" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A162" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -8011,7 +8006,7 @@
     </row>
     <row r="163" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A163" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -8056,7 +8051,7 @@
     </row>
     <row r="164" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A164" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -8101,7 +8096,7 @@
     </row>
     <row r="165" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A165" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B165">
         <v>0</v>
@@ -8146,7 +8141,7 @@
     </row>
     <row r="166" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A166" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -8194,7 +8189,7 @@
     </row>
     <row r="167" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A167" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -8239,7 +8234,7 @@
     </row>
     <row r="168" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A168" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -8284,7 +8279,7 @@
     </row>
     <row r="169" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A169" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -8329,7 +8324,7 @@
     </row>
     <row r="170" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A170" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B170">
         <v>0</v>
@@ -8374,7 +8369,7 @@
     </row>
     <row r="171" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A171" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -8419,7 +8414,7 @@
     </row>
     <row r="172" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A172" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -8464,7 +8459,7 @@
     </row>
     <row r="173" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A173" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -8509,7 +8504,7 @@
     </row>
     <row r="174" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A174" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B174">
         <v>0</v>
@@ -8554,7 +8549,7 @@
     </row>
     <row r="175" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A175" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B175">
         <v>0</v>
@@ -8599,7 +8594,7 @@
     </row>
     <row r="176" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A176" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -8647,7 +8642,7 @@
     </row>
     <row r="177" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A177" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -8692,7 +8687,7 @@
     </row>
     <row r="178" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A178" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -8737,7 +8732,7 @@
     </row>
     <row r="179" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A179" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B179">
         <v>0</v>
@@ -8782,7 +8777,7 @@
     </row>
     <row r="180" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A180" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B180">
         <v>0</v>
@@ -8830,7 +8825,7 @@
     </row>
     <row r="181" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A181" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B181">
         <v>0</v>
@@ -8875,7 +8870,7 @@
     </row>
     <row r="182" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A182" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -8920,7 +8915,7 @@
     </row>
     <row r="183" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A183" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B183">
         <v>0</v>
@@ -8965,7 +8960,7 @@
     </row>
     <row r="184" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A184" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B184">
         <v>0</v>
@@ -9013,7 +9008,7 @@
     </row>
     <row r="185" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A185" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B185">
         <v>0</v>
@@ -9058,7 +9053,7 @@
     </row>
     <row r="186" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A186" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B186">
         <v>0</v>
@@ -9103,7 +9098,7 @@
     </row>
     <row r="187" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A187" s="6">
-        <v>75049</v>
+        <v>42177</v>
       </c>
       <c r="B187">
         <v>0</v>

</xml_diff>